<commit_message>
Add 2015.12.28 Problems Happen List.
</commit_message>
<xml_diff>
--- a/Regression 2015-12-16.xlsx
+++ b/Regression 2015-12-16.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="No Web Engine" sheetId="1" r:id="rId1"/>
     <sheet name="Web Engine Involve" sheetId="2" r:id="rId2"/>
     <sheet name="2015.12.18 Summary" sheetId="3" r:id="rId3"/>
+    <sheet name="2015.12.28 Problems Happen List" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="68">
   <si>
     <t>IE</t>
   </si>
@@ -234,12 +235,27 @@
   <si>
     <t>AutoItTests</t>
   </si>
+  <si>
+    <t>known</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>On going</t>
+  </si>
+  <si>
+    <t>Has added Comments</t>
+  </si>
+  <si>
+    <t>No issue, but failed before</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -308,8 +324,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -337,6 +374,21 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -480,14 +532,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -556,6 +611,7 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -571,13 +627,18 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="6"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="8">
+    <cellStyle name="Bad" xfId="6" builtinId="27"/>
+    <cellStyle name="Good" xfId="5" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Input" xfId="3" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="7" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -882,8 +943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,11 +969,11 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="29"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="30"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="28" t="s">
         <v>62</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -920,8 +981,8 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="28"/>
-      <c r="B5" s="29"/>
+      <c r="A5" s="29"/>
+      <c r="B5" s="30"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
@@ -932,8 +993,8 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="28"/>
-      <c r="B7" s="29"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="30"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
@@ -957,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,12 +1057,12 @@
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="32"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
@@ -1025,12 +1086,12 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="32"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="33"/>
       <c r="H4" s="2" t="s">
         <v>43</v>
       </c>
@@ -1054,12 +1115,12 @@
       <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="32"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="33"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
@@ -1112,12 +1173,12 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="32"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="33"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="20" t="s">
@@ -1162,12 +1223,12 @@
       <c r="F13" s="12"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="32"/>
+      <c r="A14" s="31"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="33"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="20" t="s">
@@ -1206,12 +1267,12 @@
       <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="32"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="33"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
@@ -1256,12 +1317,12 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="32"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="33"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="20" t="s">
@@ -1306,12 +1367,12 @@
       <c r="F24" s="12"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="32"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="33"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="20" t="s">
@@ -1356,12 +1417,12 @@
       <c r="F28" s="12"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="32"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="33"/>
     </row>
     <row r="30" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="20" t="s">
@@ -1432,12 +1493,12 @@
       <c r="F33" s="12"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="32"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="33"/>
     </row>
     <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="20" t="s">
@@ -1454,12 +1515,12 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="32"/>
+      <c r="A36" s="31"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="33"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
@@ -1504,12 +1565,12 @@
       <c r="F39" s="12"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="30"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="32"/>
+      <c r="A40" s="31"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="33"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="20" t="s">
@@ -1619,11 +1680,11 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
@@ -1643,11 +1704,11 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
@@ -1667,11 +1728,11 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="31"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="31"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
     </row>
     <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
@@ -1691,11 +1752,11 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
     </row>
     <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
@@ -1726,4 +1787,201 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="49.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="12"/>
+      <c r="G3" s="36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="35" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="B3" r:id="rId2"/>
+    <hyperlink ref="B5" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update the status of 'dragTo'.
</commit_message>
<xml_diff>
--- a/Regression 2015-12-16.xlsx
+++ b/Regression 2015-12-16.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="69">
   <si>
     <t>IE</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>No issue, but failed before</t>
+  </si>
+  <si>
+    <t>Test Cases</t>
   </si>
 </sst>
 </file>
@@ -627,9 +630,9 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="4" xfId="7" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" xfId="5" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Bad" xfId="6" builtinId="27"/>
@@ -1019,7 +1022,7 @@
   <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1794,7 +1797,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1808,6 +1811,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="B1" s="5" t="s">
         <v>6</v>
       </c>
@@ -1827,132 +1833,132 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="12"/>
+      <c r="G2" s="34" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B3" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="27" t="s">
+      <c r="C3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G3" s="35" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="36" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="12"/>
-      <c r="G4" s="34" t="s">
+      <c r="D5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="35" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="12"/>
-      <c r="G5" s="36" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>36</v>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>5</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>5</v>
       </c>
       <c r="F6" s="12"/>
       <c r="G6" s="35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="36" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="34" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1972,16 +1978,17 @@
         <v>5</v>
       </c>
       <c r="F8" s="12"/>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="36" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>